<commit_message>
Update GARP.xlsx with latest data
</commit_message>
<xml_diff>
--- a/GARP.xlsx
+++ b/GARP.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,419 +463,419 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lumax Auto Tech.</t>
+          <t>Krishana Phosch.</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1090</v>
+        <v>521.75</v>
       </c>
       <c r="C2" t="n">
-        <v>103.3</v>
+        <v>92.19</v>
       </c>
       <c r="D2" t="n">
-        <v>105.31</v>
+        <v>160.47</v>
       </c>
       <c r="E2" t="n">
-        <v>90.29000000000001</v>
+        <v>92.70999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Krishana Phosch.</t>
+          <t>Lumax Auto Tech.</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>521.75</v>
+        <v>1090</v>
       </c>
       <c r="C3" t="n">
-        <v>92.19</v>
+        <v>103.3</v>
       </c>
       <c r="D3" t="n">
-        <v>160.47</v>
+        <v>105.31</v>
       </c>
       <c r="E3" t="n">
-        <v>92.70999999999999</v>
+        <v>90.29000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Banco Products</t>
+          <t>Aditya Birla Cap</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>638.95</v>
+        <v>270.95</v>
       </c>
       <c r="C4" t="n">
-        <v>65.02</v>
+        <v>38.28</v>
       </c>
       <c r="D4" t="n">
-        <v>47.99</v>
+        <v>58.98</v>
       </c>
       <c r="E4" t="n">
-        <v>85.06999999999999</v>
+        <v>25.73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pearl Global Ind</t>
+          <t>ITD Cem</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1545.3</v>
+        <v>787.6</v>
       </c>
       <c r="C5" t="n">
-        <v>57.22</v>
+        <v>51.93</v>
       </c>
       <c r="D5" t="n">
-        <v>18.51</v>
+        <v>53.35</v>
       </c>
       <c r="E5" t="n">
-        <v>75.34999999999999</v>
+        <v>54.27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Dynamic Cables</t>
+          <t>Banco Products</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>432.25</v>
+        <v>638.95</v>
       </c>
       <c r="C6" t="n">
-        <v>56.26</v>
+        <v>65.02</v>
       </c>
       <c r="D6" t="n">
-        <v>1.04</v>
+        <v>47.99</v>
       </c>
       <c r="E6" t="n">
-        <v>45.91</v>
+        <v>85.06999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lloyds Enterpris</t>
+          <t>Multi Comm. Exc.</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>81.52</v>
+        <v>8242.5</v>
       </c>
       <c r="C7" t="n">
-        <v>53.67</v>
+        <v>36.18</v>
       </c>
       <c r="D7" t="n">
-        <v>37.38</v>
+        <v>43.61</v>
       </c>
       <c r="E7" t="n">
-        <v>127.2</v>
+        <v>102.69</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ITD Cem</t>
+          <t>Chola Financial</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>787.6</v>
+        <v>2046.7</v>
       </c>
       <c r="C8" t="n">
-        <v>51.93</v>
+        <v>3.35</v>
       </c>
       <c r="D8" t="n">
-        <v>53.35</v>
+        <v>43.47</v>
       </c>
       <c r="E8" t="n">
-        <v>54.27</v>
+        <v>36.83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Aditya Birla Cap</t>
+          <t>Home First Finan</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>270.95</v>
+        <v>1415.9</v>
       </c>
       <c r="C9" t="n">
-        <v>38.28</v>
+        <v>14.69</v>
       </c>
       <c r="D9" t="n">
-        <v>58.98</v>
+        <v>42.17</v>
       </c>
       <c r="E9" t="n">
-        <v>25.73</v>
+        <v>35.94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fedbank Financi.</t>
+          <t>Lloyds Enterpris</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>123.72</v>
+        <v>81.52</v>
       </c>
       <c r="C10" t="n">
-        <v>37.51</v>
+        <v>53.67</v>
       </c>
       <c r="D10" t="n">
-        <v>29.84</v>
+        <v>37.38</v>
       </c>
       <c r="E10" t="n">
-        <v>0.55</v>
+        <v>127.2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Multi Comm. Exc.</t>
+          <t>Kalyan Jewellers</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8242.5</v>
+        <v>613</v>
       </c>
       <c r="C11" t="n">
-        <v>36.18</v>
+        <v>22.29</v>
       </c>
       <c r="D11" t="n">
-        <v>43.61</v>
+        <v>33.62</v>
       </c>
       <c r="E11" t="n">
-        <v>102.69</v>
+        <v>4.38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Gokul Agro</t>
+          <t>BSE</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>314.25</v>
+        <v>2547.8</v>
       </c>
       <c r="C12" t="n">
-        <v>28.19</v>
+        <v>21.26</v>
       </c>
       <c r="D12" t="n">
-        <v>5.7</v>
+        <v>30.98</v>
       </c>
       <c r="E12" t="n">
-        <v>84.26000000000001</v>
+        <v>216.69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Genus Power</t>
+          <t>TD Power Systems</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>373.2</v>
+        <v>480.1</v>
       </c>
       <c r="C13" t="n">
-        <v>24.82</v>
+        <v>14.9</v>
       </c>
       <c r="D13" t="n">
-        <v>11.27</v>
+        <v>30.37</v>
       </c>
       <c r="E13" t="n">
-        <v>3.04</v>
+        <v>20.67</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Polycab India</t>
+          <t>SBFC Finance</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6841</v>
+        <v>114.49</v>
       </c>
       <c r="C14" t="n">
-        <v>24.22</v>
+        <v>7.86</v>
       </c>
       <c r="D14" t="n">
-        <v>15.64</v>
+        <v>29.87</v>
       </c>
       <c r="E14" t="n">
-        <v>8.210000000000001</v>
+        <v>39.93</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Kingfa Science</t>
+          <t>Fedbank Financi.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3654</v>
+        <v>123.72</v>
       </c>
       <c r="C15" t="n">
-        <v>23.24</v>
+        <v>37.51</v>
       </c>
       <c r="D15" t="n">
-        <v>22.43</v>
+        <v>29.84</v>
       </c>
       <c r="E15" t="n">
-        <v>43.58</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kalyan Jewellers</t>
+          <t>Bajaj Finance</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>613</v>
+        <v>958.95</v>
       </c>
       <c r="C16" t="n">
-        <v>22.29</v>
+        <v>5.24</v>
       </c>
       <c r="D16" t="n">
-        <v>33.62</v>
+        <v>28.92</v>
       </c>
       <c r="E16" t="n">
-        <v>4.38</v>
+        <v>45.14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BSE</t>
+          <t>Cholaman.Inv.&amp;Fn</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2547.8</v>
+        <v>1551.4</v>
       </c>
       <c r="C17" t="n">
-        <v>21.26</v>
+        <v>0.51</v>
       </c>
       <c r="D17" t="n">
-        <v>30.98</v>
+        <v>26.85</v>
       </c>
       <c r="E17" t="n">
-        <v>216.69</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Uno Minda</t>
+          <t>AU Small Finance</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1081</v>
+        <v>745.45</v>
       </c>
       <c r="C18" t="n">
-        <v>21.18</v>
+        <v>10.41</v>
       </c>
       <c r="D18" t="n">
-        <v>18.32</v>
+        <v>25.36</v>
       </c>
       <c r="E18" t="n">
-        <v>5.62</v>
+        <v>13.02</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>D.P. Abhushan</t>
+          <t>Suzlon Energy</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1674.7</v>
+        <v>65.31999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>16.45</v>
+        <v>12.04</v>
       </c>
       <c r="D19" t="n">
-        <v>0.08</v>
+        <v>24.32</v>
       </c>
       <c r="E19" t="n">
-        <v>27.44</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TD Power Systems</t>
+          <t>Kingfa Science</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>480.1</v>
+        <v>3654</v>
       </c>
       <c r="C20" t="n">
-        <v>14.9</v>
+        <v>23.24</v>
       </c>
       <c r="D20" t="n">
-        <v>30.37</v>
+        <v>22.43</v>
       </c>
       <c r="E20" t="n">
-        <v>20.67</v>
+        <v>43.58</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Home First Finan</t>
+          <t>Pearl Global Ind</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1415.9</v>
+        <v>1545.3</v>
       </c>
       <c r="C21" t="n">
-        <v>14.69</v>
+        <v>57.22</v>
       </c>
       <c r="D21" t="n">
-        <v>42.17</v>
+        <v>18.51</v>
       </c>
       <c r="E21" t="n">
-        <v>35.94</v>
+        <v>75.34999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Suzlon Energy</t>
+          <t>Uno Minda</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>65.31999999999999</v>
+        <v>1081</v>
       </c>
       <c r="C22" t="n">
-        <v>12.04</v>
+        <v>21.18</v>
       </c>
       <c r="D22" t="n">
-        <v>24.32</v>
+        <v>18.32</v>
       </c>
       <c r="E22" t="n">
-        <v>7.58</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AU Small Finance</t>
+          <t>Polycab India</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>745.45</v>
+        <v>6841</v>
       </c>
       <c r="C23" t="n">
-        <v>10.41</v>
+        <v>24.22</v>
       </c>
       <c r="D23" t="n">
-        <v>25.36</v>
+        <v>15.64</v>
       </c>
       <c r="E23" t="n">
-        <v>13.02</v>
+        <v>8.210000000000001</v>
       </c>
     </row>
     <row r="24">
@@ -900,20 +900,20 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SBFC Finance</t>
+          <t>Genus Power</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>114.49</v>
+        <v>373.2</v>
       </c>
       <c r="C25" t="n">
-        <v>7.86</v>
+        <v>24.82</v>
       </c>
       <c r="D25" t="n">
-        <v>29.87</v>
+        <v>11.27</v>
       </c>
       <c r="E25" t="n">
-        <v>39.93</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="26">
@@ -938,58 +938,58 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>V2 Retail</t>
+          <t>Gokul Agro</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1945.9</v>
+        <v>314.25</v>
       </c>
       <c r="C27" t="n">
-        <v>5.85</v>
+        <v>28.19</v>
       </c>
       <c r="D27" t="n">
         <v>5.7</v>
       </c>
       <c r="E27" t="n">
-        <v>142.04</v>
+        <v>84.26000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bajaj Finance</t>
+          <t>V2 Retail</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>958.95</v>
+        <v>1945.9</v>
       </c>
       <c r="C28" t="n">
-        <v>5.24</v>
+        <v>5.85</v>
       </c>
       <c r="D28" t="n">
-        <v>28.92</v>
+        <v>5.7</v>
       </c>
       <c r="E28" t="n">
-        <v>45.14</v>
+        <v>142.04</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Chola Financial</t>
+          <t>Dynamic Cables</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2046.7</v>
+        <v>432.25</v>
       </c>
       <c r="C29" t="n">
-        <v>3.35</v>
+        <v>56.26</v>
       </c>
       <c r="D29" t="n">
-        <v>43.47</v>
+        <v>1.04</v>
       </c>
       <c r="E29" t="n">
-        <v>36.83</v>
+        <v>45.91</v>
       </c>
     </row>
     <row r="30">
@@ -1014,20 +1014,20 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cholaman.Inv.&amp;Fn</t>
+          <t>D.P. Abhushan</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1551.4</v>
+        <v>1674.7</v>
       </c>
       <c r="C31" t="n">
-        <v>0.51</v>
+        <v>16.45</v>
       </c>
       <c r="D31" t="n">
-        <v>26.85</v>
+        <v>0.08</v>
       </c>
       <c r="E31" t="n">
-        <v>11.7</v>
+        <v>27.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>